<commit_message>
Maj Excel des Tables de la BDD
Ajout de la table Groupes
Ajout des clés primaires et étrangères
</commit_message>
<xml_diff>
--- a/Documentation/BDD/Tables de la BDD.xlsx
+++ b/Documentation/BDD/Tables de la BDD.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thunder\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="92">
   <si>
     <t>v_prenom</t>
   </si>
@@ -41,36 +39,15 @@
     <t>d_maj</t>
   </si>
   <si>
-    <t>v_id_emarg</t>
-  </si>
-  <si>
-    <t>v_id_etu</t>
-  </si>
-  <si>
-    <t>v_id_user</t>
-  </si>
-  <si>
-    <t>v_id_carte</t>
-  </si>
-  <si>
     <t>Creneaux</t>
   </si>
   <si>
-    <t>v_id_creneau</t>
-  </si>
-  <si>
     <t>d_debut</t>
   </si>
   <si>
     <t>d_fin</t>
   </si>
   <si>
-    <t>v_user_creat</t>
-  </si>
-  <si>
-    <t>v_user_maj</t>
-  </si>
-  <si>
     <t>v_statut</t>
   </si>
   <si>
@@ -83,9 +60,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>v_id_classe</t>
-  </si>
-  <si>
     <t>varchar(1)</t>
   </si>
   <si>
@@ -116,9 +90,6 @@
     <t>Date de création de l'étudiant</t>
   </si>
   <si>
-    <t>v_id_user_creat</t>
-  </si>
-  <si>
     <t>Identifiant de l'utilisateur ayant créé l'étudiant</t>
   </si>
   <si>
@@ -224,9 +195,6 @@
     <t>Absences</t>
   </si>
   <si>
-    <t>v_id_abs</t>
-  </si>
-  <si>
     <t>d_abs</t>
   </si>
   <si>
@@ -255,13 +223,88 @@
   </si>
   <si>
     <t>Statut de l'absence</t>
+  </si>
+  <si>
+    <t>Groupes</t>
+  </si>
+  <si>
+    <t>Identifiant du groupe</t>
+  </si>
+  <si>
+    <t>Identifiant de la classe englobant le groupe</t>
+  </si>
+  <si>
+    <t>Libelle du groupe</t>
+  </si>
+  <si>
+    <t>Date de création du groupe</t>
+  </si>
+  <si>
+    <t>Identifiant de l'utilisateur ayant créé le groupe</t>
+  </si>
+  <si>
+    <t>Date de dernière mise à jour du groupe</t>
+  </si>
+  <si>
+    <t>Identifiant de l'utilisateur ayant mis à jour le groupe</t>
+  </si>
+  <si>
+    <t>Statut du groupe</t>
+  </si>
+  <si>
+    <t>* v_id_etu</t>
+  </si>
+  <si>
+    <t>* v_id_classe</t>
+  </si>
+  <si>
+    <t>$ v_id_classe</t>
+  </si>
+  <si>
+    <t>* v_id_carte</t>
+  </si>
+  <si>
+    <t>* v_id_creneau</t>
+  </si>
+  <si>
+    <t>* v_id_groupes</t>
+  </si>
+  <si>
+    <t>* v_id_emarg</t>
+  </si>
+  <si>
+    <t>$ v_id_carte</t>
+  </si>
+  <si>
+    <t>* v_id_abs</t>
+  </si>
+  <si>
+    <t>$ v_id_etu</t>
+  </si>
+  <si>
+    <t>* v_id_user</t>
+  </si>
+  <si>
+    <t>$ v_id_user_creat</t>
+  </si>
+  <si>
+    <t>$ v_user_maj</t>
+  </si>
+  <si>
+    <t>$ v_user_creat</t>
+  </si>
+  <si>
+    <t>* = Clé primaire</t>
+  </si>
+  <si>
+    <t>$ = Clé étrangère</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,6 +320,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -286,7 +345,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -296,22 +355,22 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -321,7 +380,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -329,36 +388,36 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -366,10 +425,10 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -378,29 +437,29 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -408,22 +467,39 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -441,8 +517,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -501,7 +584,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -536,7 +619,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -713,7 +796,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -721,534 +804,632 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H34"/>
+  <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
-    <col min="8" max="8" width="49.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="49.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="49.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="15" thickBot="1"/>
+    <row r="2" spans="2:8" ht="15" thickBot="1">
       <c r="B2" s="5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>24</v>
-      </c>
       <c r="F3" s="9" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="15" thickBot="1">
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="15" thickBot="1">
       <c r="B11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="15" thickBot="1">
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
+      <c r="H12" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F13" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="2:8">
+      <c r="F13" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="15" thickBot="1">
       <c r="F14" s="9" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="15" thickBot="1">
       <c r="B15" s="5" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8">
       <c r="B17" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
       <c r="B18" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="15" thickBot="1">
+      <c r="B20" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15" thickBot="1">
+      <c r="B22" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="15" thickBot="1">
+      <c r="F23" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="15" thickBot="1">
+      <c r="F24" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="15" thickBot="1">
+      <c r="B25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="9" t="s">
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="F27" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="G27" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="15" thickBot="1">
+      <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F23" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F24" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="D28" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
       <c r="B29" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="15" thickBot="1">
       <c r="B30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="15" thickBot="1">
       <c r="B31" s="1" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8">
       <c r="B32" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8">
       <c r="B33" s="1" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="C33" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="2:8" ht="15" thickBot="1">
       <c r="B34" s="3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>42</v>
+        <v>33</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="F35" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="15" thickBot="1">
+      <c r="B36" t="s">
+        <v>90</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout des .sql de création des tables
Ajout d’un .sql par table dans la BDD + mise à jour du Excel de
description de la base
</commit_message>
<xml_diff>
--- a/Documentation/BDD/Tables de la BDD.xlsx
+++ b/Documentation/BDD/Tables de la BDD.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="93">
   <si>
     <t>v_prenom</t>
   </si>
@@ -261,15 +261,9 @@
     <t>$ v_id_classe</t>
   </si>
   <si>
-    <t>* v_id_carte</t>
-  </si>
-  <si>
     <t>* v_id_creneau</t>
   </si>
   <si>
-    <t>* v_id_groupes</t>
-  </si>
-  <si>
     <t>* v_id_emarg</t>
   </si>
   <si>
@@ -298,6 +292,15 @@
   </si>
   <si>
     <t>$ = Clé étrangère</t>
+  </si>
+  <si>
+    <t>v_id_carte</t>
+  </si>
+  <si>
+    <t>* v_id_groupe</t>
+  </si>
+  <si>
+    <t>$ v_id_groupe</t>
   </si>
 </sst>
 </file>
@@ -796,7 +799,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -806,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -865,7 +868,7 @@
     </row>
     <row r="4" spans="2:8">
       <c r="B4" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>9</v>
@@ -914,7 +917,7 @@
         <v>19</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>9</v>
@@ -925,7 +928,7 @@
     </row>
     <row r="7" spans="2:8">
       <c r="B7" s="1" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>9</v>
@@ -954,7 +957,7 @@
         <v>21</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>9</v>
@@ -965,7 +968,7 @@
     </row>
     <row r="9" spans="2:8" ht="15" thickBot="1">
       <c r="B9" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>9</v>
@@ -996,7 +999,7 @@
     </row>
     <row r="11" spans="2:8" ht="15" thickBot="1">
       <c r="B11" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>9</v>
@@ -1027,7 +1030,7 @@
     </row>
     <row r="13" spans="2:8">
       <c r="F13" s="9" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>9</v>
@@ -1069,7 +1072,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>9</v>
@@ -1098,7 +1101,7 @@
         <v>18</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>9</v>
@@ -1138,7 +1141,7 @@
         <v>49</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>9</v>
@@ -1202,7 +1205,7 @@
     </row>
     <row r="24" spans="2:8" ht="15" thickBot="1">
       <c r="F24" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>9</v>
@@ -1222,7 +1225,7 @@
         <v>15</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>9</v>
@@ -1233,7 +1236,7 @@
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>9</v>
@@ -1253,7 +1256,7 @@
     </row>
     <row r="27" spans="2:8">
       <c r="B27" s="1" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>9</v>
@@ -1315,7 +1318,7 @@
     </row>
     <row r="31" spans="2:8" ht="15" thickBot="1">
       <c r="B31" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>9</v>
@@ -1344,7 +1347,7 @@
         <v>32</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G32" s="7" t="s">
         <v>9</v>
@@ -1355,7 +1358,7 @@
     </row>
     <row r="33" spans="2:8">
       <c r="B33" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>9</v>
@@ -1364,7 +1367,7 @@
         <v>31</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G33" s="7" t="s">
         <v>9</v>
@@ -1406,7 +1409,7 @@
     </row>
     <row r="36" spans="2:8" ht="15" thickBot="1">
       <c r="B36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F36" s="15" t="s">
         <v>8</v>
@@ -1420,12 +1423,11 @@
     </row>
     <row r="37" spans="2:8">
       <c r="B37" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>